<commit_message>
Add new FSH files for September Connectathon
</commit_message>
<xml_diff>
--- a/build/output/StructureDefinition-pacio-plcf.xlsx
+++ b/build/output/StructureDefinition-pacio-plcf.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AO$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AO$57</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1980" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2129" uniqueCount="448">
   <si>
     <t>Path</t>
   </si>
@@ -592,7 +592,13 @@
     <t>Knowing what kind of observation is being made is essential to understanding the observation.</t>
   </si>
   <si>
-    <t>extensible</t>
+    <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
+  &lt;coding&gt;
+    &lt;system value="http://loinc.org"/&gt;
+    &lt;code value="11332-4"/&gt;
+    &lt;display value="History of Cognitive Function Narrative"/&gt;
+  &lt;/coding&gt;
+&lt;/valueCodeableConcept&gt;</t>
   </si>
   <si>
     <t>http://loinc.org</t>
@@ -614,6 +620,91 @@
   </si>
   <si>
     <t>116680003 |Is a|</t>
+  </si>
+  <si>
+    <t>Observation.code.id</t>
+  </si>
+  <si>
+    <t>Unique id for inter-element referencing</t>
+  </si>
+  <si>
+    <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
+  </si>
+  <si>
+    <t>Element.id</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>Observation.code.extension</t>
+  </si>
+  <si>
+    <t>Additional content defined by implementations</t>
+  </si>
+  <si>
+    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
+  </si>
+  <si>
+    <t>Extensions are always sliced by (at least) url</t>
+  </si>
+  <si>
+    <t>Element.extension</t>
+  </si>
+  <si>
+    <t>Observation.code.coding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coding
+</t>
+  </si>
+  <si>
+    <t>Code defined by a terminology system</t>
+  </si>
+  <si>
+    <t>A reference to a code defined by a terminology system.</t>
+  </si>
+  <si>
+    <t>Codes may be defined very casually in enumerations, or code lists, up to very formal definitions such as SNOMED CT - see the HL7 v3 Core Principles for more information.  Ordering of codings is undefined and SHALL NOT be used to infer meaning. Generally, at most only one of the coding values will be labeled as UserSelected = true.</t>
+  </si>
+  <si>
+    <t>Allows for alternative encodings within a code system, and translations to other code systems.</t>
+  </si>
+  <si>
+    <t>CodeableConcept.coding</t>
+  </si>
+  <si>
+    <t>C*E.1-8, C*E.10-22</t>
+  </si>
+  <si>
+    <t>union(., ./translation)</t>
+  </si>
+  <si>
+    <t>Observation.code.text</t>
+  </si>
+  <si>
+    <t>Plain text representation of the concept</t>
+  </si>
+  <si>
+    <t>A human language representation of the concept as seen/selected/uttered by the user who entered the data and/or which represents the intended meaning of the user.</t>
+  </si>
+  <si>
+    <t>Very often the text is the same as a displayName of one of the codings.</t>
+  </si>
+  <si>
+    <t>The codes from the terminologies do not always capture the correct meaning with all the nuances of the human using them, or sometimes there is no appropriate code at all. In these cases, the text is used to capture the full meaning of the source.</t>
+  </si>
+  <si>
+    <t>History of Cognitive Function Narrative</t>
+  </si>
+  <si>
+    <t>CodeableConcept.text</t>
+  </si>
+  <si>
+    <t>C*E.9. But note many systems use C*E.2 for this</t>
+  </si>
+  <si>
+    <t>./originalText[mediaType/code="text/plain"]/data</t>
   </si>
   <si>
     <t>Observation.subject</t>
@@ -792,6 +883,10 @@
     <t>Observation.value[x]</t>
   </si>
   <si>
+    <t>Quantity
+CodeableConceptstringbooleanintegerRangeRatioSampledDatatimedateTimePeriod</t>
+  </si>
+  <si>
     <t>Actual result</t>
   </si>
   <si>
@@ -836,6 +931,9 @@
     <t>For many results it is necessary to handle exceptional values in measurements.</t>
   </si>
   <si>
+    <t>extensible</t>
+  </si>
+  <si>
     <t>Codes specifying why the result (`Observation.value[x]`) is missing.</t>
   </si>
   <si>
@@ -1060,28 +1158,7 @@
     <t>Observation.referenceRange.id</t>
   </si>
   <si>
-    <t>Unique id for inter-element referencing</t>
-  </si>
-  <si>
-    <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
-  </si>
-  <si>
-    <t>Element.id</t>
-  </si>
-  <si>
-    <t>n/a</t>
-  </si>
-  <si>
     <t>Observation.referenceRange.extension</t>
-  </si>
-  <si>
-    <t>Additional content defined by implementations</t>
-  </si>
-  <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
-  </si>
-  <si>
-    <t>Element.extension</t>
   </si>
   <si>
     <t>Observation.referenceRange.modifierExtension</t>
@@ -1315,10 +1392,6 @@
   </si>
   <si>
     <t>Observation.component.value[x]</t>
-  </si>
-  <si>
-    <t>Quantity
-CodeableConceptstringbooleanintegerRangeRatioSampledDatatimedateTimePeriod</t>
   </si>
   <si>
     <t>Actual component result</t>
@@ -1501,7 +1574,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AO53"/>
+  <dimension ref="A1:AO57"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1537,7 +1610,7 @@
     <col min="25" max="25" width="50.40625" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="6.34765625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="22.71484375" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="20.58984375" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="42.03125" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="17.2109375" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="14.4140625" customWidth="true" bestFit="true"/>
     <col min="31" max="31" width="41.01953125" customWidth="true" bestFit="true" hidden="true"/>
@@ -3599,7 +3672,7 @@
         <v>45</v>
       </c>
       <c r="R18" t="s" s="2">
-        <v>45</v>
+        <v>183</v>
       </c>
       <c r="S18" t="s" s="2">
         <v>45</v>
@@ -3614,7 +3687,7 @@
         <v>45</v>
       </c>
       <c r="W18" t="s" s="2">
-        <v>183</v>
+        <v>159</v>
       </c>
       <c r="X18" s="2"/>
       <c r="Y18" t="s" s="2">
@@ -3679,7 +3752,7 @@
       </c>
       <c r="D19" s="2"/>
       <c r="E19" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F19" t="s" s="2">
         <v>55</v>
@@ -3691,23 +3764,19 @@
         <v>45</v>
       </c>
       <c r="I19" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J19" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="K19" t="s" s="2">
         <v>192</v>
       </c>
-      <c r="K19" t="s" s="2">
+      <c r="L19" t="s" s="2">
         <v>193</v>
       </c>
-      <c r="L19" t="s" s="2">
-        <v>194</v>
-      </c>
-      <c r="M19" t="s" s="2">
-        <v>195</v>
-      </c>
-      <c r="N19" t="s" s="2">
-        <v>196</v>
-      </c>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
       <c r="O19" t="s" s="2">
         <v>45</v>
       </c>
@@ -3755,7 +3824,7 @@
         <v>45</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>43</v>
@@ -3767,22 +3836,22 @@
         <v>45</v>
       </c>
       <c r="AI19" t="s" s="2">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>197</v>
+        <v>45</v>
       </c>
       <c r="AK19" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL19" t="s" s="2">
-        <v>198</v>
+        <v>45</v>
       </c>
       <c r="AM19" t="s" s="2">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="AN19" t="s" s="2">
-        <v>200</v>
+        <v>45</v>
       </c>
       <c r="AO19" t="s" s="2">
         <v>45</v>
@@ -3790,11 +3859,11 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
-        <v>45</v>
+        <v>121</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" t="s" s="2">
@@ -3810,19 +3879,19 @@
         <v>45</v>
       </c>
       <c r="I20" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>202</v>
+        <v>100</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>205</v>
+        <v>124</v>
       </c>
       <c r="N20" s="2"/>
       <c r="O20" t="s" s="2">
@@ -3860,19 +3929,19 @@
         <v>45</v>
       </c>
       <c r="AA20" t="s" s="2">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="AB20" t="s" s="2">
-        <v>45</v>
+        <v>199</v>
       </c>
       <c r="AC20" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD20" t="s" s="2">
-        <v>45</v>
+        <v>104</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>43</v>
@@ -3884,7 +3953,7 @@
         <v>45</v>
       </c>
       <c r="AI20" t="s" s="2">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="AJ20" t="s" s="2">
         <v>45</v>
@@ -3893,13 +3962,13 @@
         <v>45</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>187</v>
+        <v>45</v>
       </c>
       <c r="AM20" t="s" s="2">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="AN20" t="s" s="2">
-        <v>200</v>
+        <v>45</v>
       </c>
       <c r="AO20" t="s" s="2">
         <v>45</v>
@@ -3907,18 +3976,18 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
-        <v>208</v>
+        <v>45</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F21" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G21" t="s" s="2">
         <v>45</v>
@@ -3930,19 +3999,19 @@
         <v>56</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="N21" t="s" s="2">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="O21" t="s" s="2">
         <v>45</v>
@@ -3997,7 +4066,7 @@
         <v>43</v>
       </c>
       <c r="AG21" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH21" t="s" s="2">
         <v>45</v>
@@ -4006,19 +4075,19 @@
         <v>67</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>214</v>
+        <v>45</v>
       </c>
       <c r="AK21" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="AN21" t="s" s="2">
-        <v>217</v>
+        <v>45</v>
       </c>
       <c r="AO21" t="s" s="2">
         <v>45</v>
@@ -4026,11 +4095,11 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
-        <v>219</v>
+        <v>45</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" t="s" s="2">
@@ -4049,19 +4118,19 @@
         <v>56</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>220</v>
+        <v>57</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="N22" t="s" s="2">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="O22" t="s" s="2">
         <v>45</v>
@@ -4071,7 +4140,7 @@
         <v>45</v>
       </c>
       <c r="R22" t="s" s="2">
-        <v>45</v>
+        <v>215</v>
       </c>
       <c r="S22" t="s" s="2">
         <v>45</v>
@@ -4110,7 +4179,7 @@
         <v>45</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>43</v>
@@ -4125,19 +4194,19 @@
         <v>67</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>225</v>
+        <v>45</v>
       </c>
       <c r="AK22" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="AM22" t="s" s="2">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="AN22" t="s" s="2">
-        <v>228</v>
+        <v>45</v>
       </c>
       <c r="AO22" t="s" s="2">
         <v>45</v>
@@ -4145,7 +4214,7 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -4153,7 +4222,7 @@
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F23" t="s" s="2">
         <v>55</v>
@@ -4168,18 +4237,20 @@
         <v>56</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>233</v>
-      </c>
-      <c r="N23" s="2"/>
+        <v>223</v>
+      </c>
+      <c r="N23" t="s" s="2">
+        <v>224</v>
+      </c>
       <c r="O23" t="s" s="2">
         <v>45</v>
       </c>
@@ -4227,7 +4298,7 @@
         <v>45</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>43</v>
@@ -4242,19 +4313,19 @@
         <v>67</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>45</v>
+        <v>225</v>
       </c>
       <c r="AK23" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="AM23" t="s" s="2">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="AN23" t="s" s="2">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="AO23" t="s" s="2">
         <v>45</v>
@@ -4262,7 +4333,7 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -4270,7 +4341,7 @@
       </c>
       <c r="D24" s="2"/>
       <c r="E24" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F24" t="s" s="2">
         <v>44</v>
@@ -4285,18 +4356,18 @@
         <v>56</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>240</v>
-      </c>
-      <c r="M24" s="2"/>
-      <c r="N24" t="s" s="2">
-        <v>241</v>
-      </c>
+        <v>232</v>
+      </c>
+      <c r="M24" t="s" s="2">
+        <v>233</v>
+      </c>
+      <c r="N24" s="2"/>
       <c r="O24" t="s" s="2">
         <v>45</v>
       </c>
@@ -4344,7 +4415,7 @@
         <v>45</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>43</v>
@@ -4359,19 +4430,19 @@
         <v>67</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>242</v>
+        <v>45</v>
       </c>
       <c r="AK24" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>243</v>
+        <v>187</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="AN24" t="s" s="2">
-        <v>245</v>
+        <v>228</v>
       </c>
       <c r="AO24" t="s" s="2">
         <v>45</v>
@@ -4379,11 +4450,11 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
-        <v>45</v>
+        <v>236</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" t="s" s="2">
@@ -4402,19 +4473,19 @@
         <v>56</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>168</v>
+        <v>237</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="N25" t="s" s="2">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="O25" t="s" s="2">
         <v>45</v>
@@ -4463,7 +4534,7 @@
         <v>45</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>43</v>
@@ -4472,41 +4543,41 @@
         <v>55</v>
       </c>
       <c r="AH25" t="s" s="2">
-        <v>251</v>
+        <v>45</v>
       </c>
       <c r="AI25" t="s" s="2">
         <v>67</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>45</v>
+        <v>242</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>252</v>
+        <v>45</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="AM25" t="s" s="2">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="AN25" t="s" s="2">
-        <v>45</v>
+        <v>245</v>
       </c>
       <c r="AO25" t="s" s="2">
-        <v>255</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
-        <v>45</v>
+        <v>247</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F26" t="s" s="2">
         <v>55</v>
@@ -4518,22 +4589,22 @@
         <v>45</v>
       </c>
       <c r="I26" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>168</v>
+        <v>248</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="N26" t="s" s="2">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="O26" t="s" s="2">
         <v>45</v>
@@ -4558,13 +4629,13 @@
         <v>45</v>
       </c>
       <c r="W26" t="s" s="2">
-        <v>183</v>
+        <v>45</v>
       </c>
       <c r="X26" t="s" s="2">
-        <v>261</v>
+        <v>45</v>
       </c>
       <c r="Y26" t="s" s="2">
-        <v>262</v>
+        <v>45</v>
       </c>
       <c r="Z26" t="s" s="2">
         <v>45</v>
@@ -4582,7 +4653,7 @@
         <v>45</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>43</v>
@@ -4591,25 +4662,25 @@
         <v>55</v>
       </c>
       <c r="AH26" t="s" s="2">
-        <v>263</v>
+        <v>45</v>
       </c>
       <c r="AI26" t="s" s="2">
         <v>67</v>
       </c>
       <c r="AJ26" t="s" s="2">
-        <v>45</v>
+        <v>253</v>
       </c>
       <c r="AK26" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>98</v>
+        <v>254</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="AN26" t="s" s="2">
-        <v>45</v>
+        <v>256</v>
       </c>
       <c r="AO26" t="s" s="2">
         <v>45</v>
@@ -4617,18 +4688,18 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
-        <v>266</v>
+        <v>45</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F27" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G27" t="s" s="2">
         <v>45</v>
@@ -4637,23 +4708,21 @@
         <v>45</v>
       </c>
       <c r="I27" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>168</v>
+        <v>258</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>269</v>
-      </c>
-      <c r="N27" t="s" s="2">
-        <v>270</v>
-      </c>
+        <v>261</v>
+      </c>
+      <c r="N27" s="2"/>
       <c r="O27" t="s" s="2">
         <v>45</v>
       </c>
@@ -4677,13 +4746,13 @@
         <v>45</v>
       </c>
       <c r="W27" t="s" s="2">
-        <v>183</v>
+        <v>45</v>
       </c>
       <c r="X27" t="s" s="2">
-        <v>271</v>
+        <v>45</v>
       </c>
       <c r="Y27" t="s" s="2">
-        <v>272</v>
+        <v>45</v>
       </c>
       <c r="Z27" t="s" s="2">
         <v>45</v>
@@ -4701,13 +4770,13 @@
         <v>45</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG27" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH27" t="s" s="2">
         <v>45</v>
@@ -4719,24 +4788,24 @@
         <v>45</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>273</v>
+        <v>45</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="AN27" t="s" s="2">
-        <v>45</v>
+        <v>264</v>
       </c>
       <c r="AO27" t="s" s="2">
-        <v>276</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>277</v>
+        <v>265</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4744,7 +4813,7 @@
       </c>
       <c r="D28" s="2"/>
       <c r="E28" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F28" t="s" s="2">
         <v>44</v>
@@ -4756,22 +4825,20 @@
         <v>45</v>
       </c>
       <c r="I28" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>278</v>
+        <v>266</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>279</v>
+        <v>267</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>280</v>
-      </c>
-      <c r="M28" t="s" s="2">
-        <v>281</v>
-      </c>
+        <v>268</v>
+      </c>
+      <c r="M28" s="2"/>
       <c r="N28" t="s" s="2">
-        <v>282</v>
+        <v>269</v>
       </c>
       <c r="O28" t="s" s="2">
         <v>45</v>
@@ -4820,7 +4887,7 @@
         <v>45</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>277</v>
+        <v>265</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>43</v>
@@ -4835,19 +4902,19 @@
         <v>67</v>
       </c>
       <c r="AJ28" t="s" s="2">
-        <v>45</v>
+        <v>270</v>
       </c>
       <c r="AK28" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>283</v>
+        <v>271</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="AN28" t="s" s="2">
-        <v>45</v>
+        <v>273</v>
       </c>
       <c r="AO28" t="s" s="2">
         <v>45</v>
@@ -4855,7 +4922,7 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4875,21 +4942,23 @@
         <v>45</v>
       </c>
       <c r="I29" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>168</v>
+        <v>275</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>288</v>
-      </c>
-      <c r="N29" s="2"/>
+        <v>278</v>
+      </c>
+      <c r="N29" t="s" s="2">
+        <v>279</v>
+      </c>
       <c r="O29" t="s" s="2">
         <v>45</v>
       </c>
@@ -4913,13 +4982,13 @@
         <v>45</v>
       </c>
       <c r="W29" t="s" s="2">
-        <v>289</v>
+        <v>45</v>
       </c>
       <c r="X29" t="s" s="2">
-        <v>290</v>
+        <v>45</v>
       </c>
       <c r="Y29" t="s" s="2">
-        <v>291</v>
+        <v>45</v>
       </c>
       <c r="Z29" t="s" s="2">
         <v>45</v>
@@ -4937,7 +5006,7 @@
         <v>45</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>43</v>
@@ -4946,7 +5015,7 @@
         <v>55</v>
       </c>
       <c r="AH29" t="s" s="2">
-        <v>45</v>
+        <v>280</v>
       </c>
       <c r="AI29" t="s" s="2">
         <v>67</v>
@@ -4955,24 +5024,24 @@
         <v>45</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="AN29" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO29" t="s" s="2">
-        <v>295</v>
+        <v>284</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4998,16 +5067,16 @@
         <v>168</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="N30" t="s" s="2">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="O30" t="s" s="2">
         <v>45</v>
@@ -5032,13 +5101,13 @@
         <v>45</v>
       </c>
       <c r="W30" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="X30" t="s" s="2">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="Y30" t="s" s="2">
-        <v>302</v>
+        <v>292</v>
       </c>
       <c r="Z30" t="s" s="2">
         <v>45</v>
@@ -5056,7 +5125,7 @@
         <v>45</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>43</v>
@@ -5065,7 +5134,7 @@
         <v>55</v>
       </c>
       <c r="AH30" t="s" s="2">
-        <v>45</v>
+        <v>293</v>
       </c>
       <c r="AI30" t="s" s="2">
         <v>67</v>
@@ -5077,10 +5146,10 @@
         <v>45</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>303</v>
+        <v>98</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>304</v>
+        <v>294</v>
       </c>
       <c r="AN30" t="s" s="2">
         <v>45</v>
@@ -5091,18 +5160,18 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
-        <v>45</v>
+        <v>296</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F31" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G31" t="s" s="2">
         <v>45</v>
@@ -5114,18 +5183,20 @@
         <v>45</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>306</v>
+        <v>168</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>309</v>
-      </c>
-      <c r="N31" s="2"/>
+        <v>299</v>
+      </c>
+      <c r="N31" t="s" s="2">
+        <v>300</v>
+      </c>
       <c r="O31" t="s" s="2">
         <v>45</v>
       </c>
@@ -5149,13 +5220,13 @@
         <v>45</v>
       </c>
       <c r="W31" t="s" s="2">
-        <v>45</v>
+        <v>290</v>
       </c>
       <c r="X31" t="s" s="2">
-        <v>45</v>
+        <v>301</v>
       </c>
       <c r="Y31" t="s" s="2">
-        <v>45</v>
+        <v>302</v>
       </c>
       <c r="Z31" t="s" s="2">
         <v>45</v>
@@ -5173,13 +5244,13 @@
         <v>45</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG31" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH31" t="s" s="2">
         <v>45</v>
@@ -5191,24 +5262,24 @@
         <v>45</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="AN31" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO31" t="s" s="2">
-        <v>313</v>
+        <v>306</v>
       </c>
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -5219,7 +5290,7 @@
         <v>43</v>
       </c>
       <c r="F32" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G32" t="s" s="2">
         <v>45</v>
@@ -5231,18 +5302,20 @@
         <v>45</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>318</v>
-      </c>
-      <c r="N32" s="2"/>
+        <v>311</v>
+      </c>
+      <c r="N32" t="s" s="2">
+        <v>312</v>
+      </c>
       <c r="O32" t="s" s="2">
         <v>45</v>
       </c>
@@ -5290,13 +5363,13 @@
         <v>45</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG32" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH32" t="s" s="2">
         <v>45</v>
@@ -5308,24 +5381,24 @@
         <v>45</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>319</v>
+        <v>45</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO32" t="s" s="2">
-        <v>322</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -5336,7 +5409,7 @@
         <v>43</v>
       </c>
       <c r="F33" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G33" t="s" s="2">
         <v>45</v>
@@ -5348,20 +5421,18 @@
         <v>45</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>324</v>
+        <v>168</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>327</v>
-      </c>
-      <c r="N33" t="s" s="2">
-        <v>328</v>
-      </c>
+        <v>318</v>
+      </c>
+      <c r="N33" s="2"/>
       <c r="O33" t="s" s="2">
         <v>45</v>
       </c>
@@ -5385,13 +5456,13 @@
         <v>45</v>
       </c>
       <c r="W33" t="s" s="2">
-        <v>45</v>
+        <v>319</v>
       </c>
       <c r="X33" t="s" s="2">
-        <v>45</v>
+        <v>320</v>
       </c>
       <c r="Y33" t="s" s="2">
-        <v>45</v>
+        <v>321</v>
       </c>
       <c r="Z33" t="s" s="2">
         <v>45</v>
@@ -5409,42 +5480,42 @@
         <v>45</v>
       </c>
       <c r="AE33" t="s" s="2">
+        <v>315</v>
+      </c>
+      <c r="AF33" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG33" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AH33" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI33" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="AJ33" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK33" t="s" s="2">
+        <v>322</v>
+      </c>
+      <c r="AL33" t="s" s="2">
         <v>323</v>
       </c>
-      <c r="AF33" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG33" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AH33" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI33" t="s" s="2">
-        <v>329</v>
-      </c>
-      <c r="AJ33" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK33" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL33" t="s" s="2">
-        <v>330</v>
-      </c>
       <c r="AM33" t="s" s="2">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="AN33" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO33" t="s" s="2">
-        <v>45</v>
+        <v>325</v>
       </c>
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -5467,16 +5538,20 @@
         <v>45</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>57</v>
+        <v>168</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>334</v>
-      </c>
-      <c r="M34" s="2"/>
-      <c r="N34" s="2"/>
+        <v>328</v>
+      </c>
+      <c r="M34" t="s" s="2">
+        <v>329</v>
+      </c>
+      <c r="N34" t="s" s="2">
+        <v>330</v>
+      </c>
       <c r="O34" t="s" s="2">
         <v>45</v>
       </c>
@@ -5500,13 +5575,13 @@
         <v>45</v>
       </c>
       <c r="W34" t="s" s="2">
-        <v>45</v>
+        <v>319</v>
       </c>
       <c r="X34" t="s" s="2">
-        <v>45</v>
+        <v>331</v>
       </c>
       <c r="Y34" t="s" s="2">
-        <v>45</v>
+        <v>332</v>
       </c>
       <c r="Z34" t="s" s="2">
         <v>45</v>
@@ -5524,7 +5599,7 @@
         <v>45</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>43</v>
@@ -5536,7 +5611,7 @@
         <v>45</v>
       </c>
       <c r="AI34" t="s" s="2">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="AJ34" t="s" s="2">
         <v>45</v>
@@ -5545,10 +5620,10 @@
         <v>45</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>45</v>
+        <v>333</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="AN34" t="s" s="2">
         <v>45</v>
@@ -5559,18 +5634,18 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
-        <v>121</v>
+        <v>45</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F35" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G35" t="s" s="2">
         <v>45</v>
@@ -5582,16 +5657,16 @@
         <v>45</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>100</v>
+        <v>336</v>
       </c>
       <c r="K35" t="s" s="2">
+        <v>337</v>
+      </c>
+      <c r="L35" t="s" s="2">
         <v>338</v>
       </c>
-      <c r="L35" t="s" s="2">
+      <c r="M35" t="s" s="2">
         <v>339</v>
-      </c>
-      <c r="M35" t="s" s="2">
-        <v>124</v>
       </c>
       <c r="N35" s="2"/>
       <c r="O35" t="s" s="2">
@@ -5641,78 +5716,76 @@
         <v>45</v>
       </c>
       <c r="AE35" t="s" s="2">
+        <v>335</v>
+      </c>
+      <c r="AF35" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG35" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AH35" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI35" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="AJ35" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK35" t="s" s="2">
         <v>340</v>
       </c>
-      <c r="AF35" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG35" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AH35" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI35" t="s" s="2">
-        <v>106</v>
-      </c>
-      <c r="AJ35" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK35" t="s" s="2">
-        <v>45</v>
-      </c>
       <c r="AL35" t="s" s="2">
-        <v>45</v>
+        <v>341</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>336</v>
+        <v>342</v>
       </c>
       <c r="AN35" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO35" t="s" s="2">
-        <v>45</v>
+        <v>343</v>
       </c>
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
-        <v>342</v>
+        <v>45</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F36" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G36" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H36" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="I36" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>100</v>
+        <v>345</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>124</v>
-      </c>
-      <c r="N36" t="s" s="2">
-        <v>125</v>
-      </c>
+        <v>348</v>
+      </c>
+      <c r="N36" s="2"/>
       <c r="O36" t="s" s="2">
         <v>45</v>
       </c>
@@ -5760,42 +5833,42 @@
         <v>45</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG36" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH36" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI36" t="s" s="2">
-        <v>106</v>
+        <v>67</v>
       </c>
       <c r="AJ36" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>45</v>
+        <v>349</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>45</v>
+        <v>350</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>98</v>
+        <v>351</v>
       </c>
       <c r="AN36" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO36" t="s" s="2">
-        <v>45</v>
+        <v>352</v>
       </c>
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5806,7 +5879,7 @@
         <v>43</v>
       </c>
       <c r="F37" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G37" t="s" s="2">
         <v>45</v>
@@ -5818,16 +5891,20 @@
         <v>45</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>347</v>
+        <v>354</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>348</v>
+        <v>355</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>349</v>
-      </c>
-      <c r="M37" s="2"/>
-      <c r="N37" s="2"/>
+        <v>356</v>
+      </c>
+      <c r="M37" t="s" s="2">
+        <v>357</v>
+      </c>
+      <c r="N37" t="s" s="2">
+        <v>358</v>
+      </c>
       <c r="O37" t="s" s="2">
         <v>45</v>
       </c>
@@ -5875,19 +5952,19 @@
         <v>45</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG37" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH37" t="s" s="2">
-        <v>350</v>
+        <v>45</v>
       </c>
       <c r="AI37" t="s" s="2">
-        <v>67</v>
+        <v>359</v>
       </c>
       <c r="AJ37" t="s" s="2">
         <v>45</v>
@@ -5896,10 +5973,10 @@
         <v>45</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>351</v>
+        <v>360</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>352</v>
+        <v>361</v>
       </c>
       <c r="AN37" t="s" s="2">
         <v>45</v>
@@ -5910,7 +5987,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>353</v>
+        <v>362</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5933,13 +6010,13 @@
         <v>45</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>347</v>
+        <v>57</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>354</v>
+        <v>192</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>355</v>
+        <v>193</v>
       </c>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -5990,7 +6067,7 @@
         <v>45</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>353</v>
+        <v>194</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>43</v>
@@ -5999,10 +6076,10 @@
         <v>55</v>
       </c>
       <c r="AH38" t="s" s="2">
-        <v>350</v>
+        <v>45</v>
       </c>
       <c r="AI38" t="s" s="2">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="AJ38" t="s" s="2">
         <v>45</v>
@@ -6011,10 +6088,10 @@
         <v>45</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>351</v>
+        <v>45</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>356</v>
+        <v>195</v>
       </c>
       <c r="AN38" t="s" s="2">
         <v>45</v>
@@ -6025,18 +6102,18 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>357</v>
+        <v>363</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
-        <v>45</v>
+        <v>121</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F39" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G39" t="s" s="2">
         <v>45</v>
@@ -6048,20 +6125,18 @@
         <v>45</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>168</v>
+        <v>100</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>358</v>
+        <v>197</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>359</v>
+        <v>198</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>360</v>
-      </c>
-      <c r="N39" t="s" s="2">
-        <v>361</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="N39" s="2"/>
       <c r="O39" t="s" s="2">
         <v>45</v>
       </c>
@@ -6085,13 +6160,13 @@
         <v>45</v>
       </c>
       <c r="W39" t="s" s="2">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="X39" t="s" s="2">
-        <v>362</v>
+        <v>45</v>
       </c>
       <c r="Y39" t="s" s="2">
-        <v>363</v>
+        <v>45</v>
       </c>
       <c r="Z39" t="s" s="2">
         <v>45</v>
@@ -6109,31 +6184,31 @@
         <v>45</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>357</v>
+        <v>200</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG39" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH39" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI39" t="s" s="2">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="AJ39" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>364</v>
+        <v>45</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>365</v>
+        <v>45</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>275</v>
+        <v>195</v>
       </c>
       <c r="AN39" t="s" s="2">
         <v>45</v>
@@ -6144,11 +6219,11 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
-        <v>45</v>
+        <v>365</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" t="s" s="2">
@@ -6161,25 +6236,25 @@
         <v>45</v>
       </c>
       <c r="H40" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="I40" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>168</v>
+        <v>100</v>
       </c>
       <c r="K40" t="s" s="2">
+        <v>366</v>
+      </c>
+      <c r="L40" t="s" s="2">
         <v>367</v>
       </c>
-      <c r="L40" t="s" s="2">
-        <v>368</v>
-      </c>
       <c r="M40" t="s" s="2">
-        <v>369</v>
+        <v>124</v>
       </c>
       <c r="N40" t="s" s="2">
-        <v>370</v>
+        <v>125</v>
       </c>
       <c r="O40" t="s" s="2">
         <v>45</v>
@@ -6204,13 +6279,13 @@
         <v>45</v>
       </c>
       <c r="W40" t="s" s="2">
-        <v>289</v>
+        <v>45</v>
       </c>
       <c r="X40" t="s" s="2">
-        <v>371</v>
+        <v>45</v>
       </c>
       <c r="Y40" t="s" s="2">
-        <v>372</v>
+        <v>45</v>
       </c>
       <c r="Z40" t="s" s="2">
         <v>45</v>
@@ -6228,7 +6303,7 @@
         <v>45</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>43</v>
@@ -6240,19 +6315,19 @@
         <v>45</v>
       </c>
       <c r="AI40" t="s" s="2">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="AJ40" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>364</v>
+        <v>45</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>365</v>
+        <v>45</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>275</v>
+        <v>98</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>45</v>
@@ -6263,7 +6338,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -6286,18 +6361,16 @@
         <v>45</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="M41" s="2"/>
-      <c r="N41" t="s" s="2">
-        <v>377</v>
-      </c>
+      <c r="N41" s="2"/>
       <c r="O41" t="s" s="2">
         <v>45</v>
       </c>
@@ -6345,7 +6418,7 @@
         <v>45</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>43</v>
@@ -6354,7 +6427,7 @@
         <v>55</v>
       </c>
       <c r="AH41" t="s" s="2">
-        <v>45</v>
+        <v>373</v>
       </c>
       <c r="AI41" t="s" s="2">
         <v>67</v>
@@ -6366,10 +6439,10 @@
         <v>45</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>45</v>
+        <v>374</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="AN41" t="s" s="2">
         <v>45</v>
@@ -6380,7 +6453,7 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6403,13 +6476,13 @@
         <v>45</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>57</v>
+        <v>370</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
@@ -6460,7 +6533,7 @@
         <v>45</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>43</v>
@@ -6469,7 +6542,7 @@
         <v>55</v>
       </c>
       <c r="AH42" t="s" s="2">
-        <v>45</v>
+        <v>373</v>
       </c>
       <c r="AI42" t="s" s="2">
         <v>67</v>
@@ -6481,10 +6554,10 @@
         <v>45</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>351</v>
+        <v>374</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="AN42" t="s" s="2">
         <v>45</v>
@@ -6495,7 +6568,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6506,7 +6579,7 @@
         <v>43</v>
       </c>
       <c r="F43" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G43" t="s" s="2">
         <v>45</v>
@@ -6515,21 +6588,23 @@
         <v>45</v>
       </c>
       <c r="I43" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J43" t="s" s="2">
+        <v>168</v>
+      </c>
+      <c r="K43" t="s" s="2">
+        <v>381</v>
+      </c>
+      <c r="L43" t="s" s="2">
+        <v>382</v>
+      </c>
+      <c r="M43" t="s" s="2">
+        <v>383</v>
+      </c>
+      <c r="N43" t="s" s="2">
         <v>384</v>
       </c>
-      <c r="K43" t="s" s="2">
-        <v>385</v>
-      </c>
-      <c r="L43" t="s" s="2">
-        <v>386</v>
-      </c>
-      <c r="M43" t="s" s="2">
-        <v>387</v>
-      </c>
-      <c r="N43" s="2"/>
       <c r="O43" t="s" s="2">
         <v>45</v>
       </c>
@@ -6553,13 +6628,13 @@
         <v>45</v>
       </c>
       <c r="W43" t="s" s="2">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="X43" t="s" s="2">
-        <v>45</v>
+        <v>385</v>
       </c>
       <c r="Y43" t="s" s="2">
-        <v>45</v>
+        <v>386</v>
       </c>
       <c r="Z43" t="s" s="2">
         <v>45</v>
@@ -6577,13 +6652,13 @@
         <v>45</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG43" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH43" t="s" s="2">
         <v>45</v>
@@ -6595,13 +6670,13 @@
         <v>45</v>
       </c>
       <c r="AK43" t="s" s="2">
-        <v>45</v>
+        <v>387</v>
       </c>
       <c r="AL43" t="s" s="2">
         <v>388</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>389</v>
+        <v>305</v>
       </c>
       <c r="AN43" t="s" s="2">
         <v>45</v>
@@ -6612,7 +6687,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6632,21 +6707,23 @@
         <v>45</v>
       </c>
       <c r="I44" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J44" t="s" s="2">
+        <v>168</v>
+      </c>
+      <c r="K44" t="s" s="2">
+        <v>390</v>
+      </c>
+      <c r="L44" t="s" s="2">
         <v>391</v>
       </c>
-      <c r="K44" t="s" s="2">
+      <c r="M44" t="s" s="2">
         <v>392</v>
       </c>
-      <c r="L44" t="s" s="2">
+      <c r="N44" t="s" s="2">
         <v>393</v>
       </c>
-      <c r="M44" t="s" s="2">
-        <v>394</v>
-      </c>
-      <c r="N44" s="2"/>
       <c r="O44" t="s" s="2">
         <v>45</v>
       </c>
@@ -6670,13 +6747,13 @@
         <v>45</v>
       </c>
       <c r="W44" t="s" s="2">
-        <v>45</v>
+        <v>319</v>
       </c>
       <c r="X44" t="s" s="2">
-        <v>45</v>
+        <v>394</v>
       </c>
       <c r="Y44" t="s" s="2">
-        <v>45</v>
+        <v>395</v>
       </c>
       <c r="Z44" t="s" s="2">
         <v>45</v>
@@ -6694,7 +6771,7 @@
         <v>45</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>43</v>
@@ -6712,13 +6789,13 @@
         <v>45</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>45</v>
+        <v>387</v>
       </c>
       <c r="AL44" t="s" s="2">
         <v>388</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>395</v>
+        <v>305</v>
       </c>
       <c r="AN44" t="s" s="2">
         <v>45</v>
@@ -6740,7 +6817,7 @@
         <v>43</v>
       </c>
       <c r="F45" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G45" t="s" s="2">
         <v>45</v>
@@ -6749,20 +6826,18 @@
         <v>45</v>
       </c>
       <c r="I45" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>324</v>
+        <v>397</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>398</v>
-      </c>
-      <c r="M45" t="s" s="2">
         <v>399</v>
       </c>
+      <c r="M45" s="2"/>
       <c r="N45" t="s" s="2">
         <v>400</v>
       </c>
@@ -6819,7 +6894,7 @@
         <v>43</v>
       </c>
       <c r="AG45" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH45" t="s" s="2">
         <v>45</v>
@@ -6834,10 +6909,10 @@
         <v>45</v>
       </c>
       <c r="AL45" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AM45" t="s" s="2">
         <v>401</v>
-      </c>
-      <c r="AM45" t="s" s="2">
-        <v>402</v>
       </c>
       <c r="AN45" t="s" s="2">
         <v>45</v>
@@ -6848,7 +6923,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6874,10 +6949,10 @@
         <v>57</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>333</v>
+        <v>403</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>334</v>
+        <v>404</v>
       </c>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
@@ -6928,7 +7003,7 @@
         <v>45</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>335</v>
+        <v>402</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>43</v>
@@ -6940,7 +7015,7 @@
         <v>45</v>
       </c>
       <c r="AI46" t="s" s="2">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="AJ46" t="s" s="2">
         <v>45</v>
@@ -6949,10 +7024,10 @@
         <v>45</v>
       </c>
       <c r="AL46" t="s" s="2">
-        <v>45</v>
+        <v>374</v>
       </c>
       <c r="AM46" t="s" s="2">
-        <v>336</v>
+        <v>405</v>
       </c>
       <c r="AN46" t="s" s="2">
         <v>45</v>
@@ -6963,11 +7038,11 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
-        <v>121</v>
+        <v>45</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" t="s" s="2">
@@ -6983,19 +7058,19 @@
         <v>45</v>
       </c>
       <c r="I47" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>100</v>
+        <v>407</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>338</v>
+        <v>408</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>339</v>
+        <v>409</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>124</v>
+        <v>410</v>
       </c>
       <c r="N47" s="2"/>
       <c r="O47" t="s" s="2">
@@ -7045,7 +7120,7 @@
         <v>45</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>340</v>
+        <v>406</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>43</v>
@@ -7057,7 +7132,7 @@
         <v>45</v>
       </c>
       <c r="AI47" t="s" s="2">
-        <v>106</v>
+        <v>67</v>
       </c>
       <c r="AJ47" t="s" s="2">
         <v>45</v>
@@ -7066,10 +7141,10 @@
         <v>45</v>
       </c>
       <c r="AL47" t="s" s="2">
-        <v>45</v>
+        <v>411</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>336</v>
+        <v>412</v>
       </c>
       <c r="AN47" t="s" s="2">
         <v>45</v>
@@ -7080,11 +7155,11 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>405</v>
+        <v>413</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
-        <v>342</v>
+        <v>45</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" t="s" s="2">
@@ -7097,26 +7172,24 @@
         <v>45</v>
       </c>
       <c r="H48" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="I48" t="s" s="2">
         <v>56</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>100</v>
+        <v>414</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>343</v>
+        <v>415</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>344</v>
+        <v>416</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>124</v>
-      </c>
-      <c r="N48" t="s" s="2">
-        <v>125</v>
-      </c>
+        <v>417</v>
+      </c>
+      <c r="N48" s="2"/>
       <c r="O48" t="s" s="2">
         <v>45</v>
       </c>
@@ -7164,7 +7237,7 @@
         <v>45</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>345</v>
+        <v>413</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>43</v>
@@ -7176,7 +7249,7 @@
         <v>45</v>
       </c>
       <c r="AI48" t="s" s="2">
-        <v>106</v>
+        <v>67</v>
       </c>
       <c r="AJ48" t="s" s="2">
         <v>45</v>
@@ -7185,10 +7258,10 @@
         <v>45</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>45</v>
+        <v>411</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>98</v>
+        <v>418</v>
       </c>
       <c r="AN48" t="s" s="2">
         <v>45</v>
@@ -7199,7 +7272,7 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>406</v>
+        <v>419</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -7207,10 +7280,10 @@
       </c>
       <c r="D49" s="2"/>
       <c r="E49" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F49" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G49" t="s" s="2">
         <v>45</v>
@@ -7222,19 +7295,19 @@
         <v>56</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>168</v>
+        <v>354</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>407</v>
+        <v>420</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>408</v>
+        <v>421</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>409</v>
+        <v>422</v>
       </c>
       <c r="N49" t="s" s="2">
-        <v>182</v>
+        <v>423</v>
       </c>
       <c r="O49" t="s" s="2">
         <v>45</v>
@@ -7259,13 +7332,13 @@
         <v>45</v>
       </c>
       <c r="W49" t="s" s="2">
-        <v>289</v>
+        <v>45</v>
       </c>
       <c r="X49" t="s" s="2">
-        <v>410</v>
+        <v>45</v>
       </c>
       <c r="Y49" t="s" s="2">
-        <v>411</v>
+        <v>45</v>
       </c>
       <c r="Z49" t="s" s="2">
         <v>45</v>
@@ -7283,13 +7356,13 @@
         <v>45</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>406</v>
+        <v>419</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="AG49" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH49" t="s" s="2">
         <v>45</v>
@@ -7301,16 +7374,16 @@
         <v>45</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>412</v>
+        <v>45</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>187</v>
+        <v>424</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>188</v>
+        <v>425</v>
       </c>
       <c r="AN49" t="s" s="2">
-        <v>189</v>
+        <v>45</v>
       </c>
       <c r="AO49" t="s" s="2">
         <v>45</v>
@@ -7318,7 +7391,7 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>413</v>
+        <v>426</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -7338,23 +7411,19 @@
         <v>45</v>
       </c>
       <c r="I50" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>414</v>
+        <v>57</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>415</v>
+        <v>192</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>248</v>
-      </c>
-      <c r="M50" t="s" s="2">
-        <v>416</v>
-      </c>
-      <c r="N50" t="s" s="2">
-        <v>250</v>
-      </c>
+        <v>193</v>
+      </c>
+      <c r="M50" s="2"/>
+      <c r="N50" s="2"/>
       <c r="O50" t="s" s="2">
         <v>45</v>
       </c>
@@ -7402,7 +7471,7 @@
         <v>45</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>413</v>
+        <v>194</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>43</v>
@@ -7414,41 +7483,41 @@
         <v>45</v>
       </c>
       <c r="AI50" t="s" s="2">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="AJ50" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>417</v>
+        <v>45</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>253</v>
+        <v>45</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>254</v>
+        <v>195</v>
       </c>
       <c r="AN50" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO50" t="s" s="2">
-        <v>255</v>
+        <v>45</v>
       </c>
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>418</v>
+        <v>427</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
-        <v>45</v>
+        <v>121</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F51" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G51" t="s" s="2">
         <v>45</v>
@@ -7460,20 +7529,18 @@
         <v>45</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>168</v>
+        <v>100</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>419</v>
+        <v>197</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>420</v>
+        <v>198</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>421</v>
-      </c>
-      <c r="N51" t="s" s="2">
-        <v>260</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="N51" s="2"/>
       <c r="O51" t="s" s="2">
         <v>45</v>
       </c>
@@ -7497,13 +7564,13 @@
         <v>45</v>
       </c>
       <c r="W51" t="s" s="2">
-        <v>183</v>
+        <v>45</v>
       </c>
       <c r="X51" t="s" s="2">
-        <v>261</v>
+        <v>45</v>
       </c>
       <c r="Y51" t="s" s="2">
-        <v>262</v>
+        <v>45</v>
       </c>
       <c r="Z51" t="s" s="2">
         <v>45</v>
@@ -7521,19 +7588,19 @@
         <v>45</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>418</v>
+        <v>200</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG51" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH51" t="s" s="2">
-        <v>263</v>
+        <v>45</v>
       </c>
       <c r="AI51" t="s" s="2">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="AJ51" t="s" s="2">
         <v>45</v>
@@ -7542,10 +7609,10 @@
         <v>45</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>98</v>
+        <v>45</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>264</v>
+        <v>195</v>
       </c>
       <c r="AN51" t="s" s="2">
         <v>45</v>
@@ -7556,11 +7623,11 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>422</v>
+        <v>428</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
-        <v>266</v>
+        <v>365</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" t="s" s="2">
@@ -7573,25 +7640,25 @@
         <v>45</v>
       </c>
       <c r="H52" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="I52" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>168</v>
+        <v>100</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>267</v>
+        <v>366</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>268</v>
+        <v>367</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>269</v>
+        <v>124</v>
       </c>
       <c r="N52" t="s" s="2">
-        <v>270</v>
+        <v>125</v>
       </c>
       <c r="O52" t="s" s="2">
         <v>45</v>
@@ -7616,13 +7683,13 @@
         <v>45</v>
       </c>
       <c r="W52" t="s" s="2">
-        <v>183</v>
+        <v>45</v>
       </c>
       <c r="X52" t="s" s="2">
-        <v>271</v>
+        <v>45</v>
       </c>
       <c r="Y52" t="s" s="2">
-        <v>272</v>
+        <v>45</v>
       </c>
       <c r="Z52" t="s" s="2">
         <v>45</v>
@@ -7640,7 +7707,7 @@
         <v>45</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>422</v>
+        <v>368</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>43</v>
@@ -7652,30 +7719,30 @@
         <v>45</v>
       </c>
       <c r="AI52" t="s" s="2">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="AJ52" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>273</v>
+        <v>45</v>
       </c>
       <c r="AL52" t="s" s="2">
-        <v>274</v>
+        <v>45</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>275</v>
+        <v>98</v>
       </c>
       <c r="AN52" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO52" t="s" s="2">
-        <v>276</v>
+        <v>45</v>
       </c>
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>423</v>
+        <v>429</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -7683,10 +7750,10 @@
       </c>
       <c r="D53" s="2"/>
       <c r="E53" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F53" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G53" t="s" s="2">
         <v>45</v>
@@ -7695,22 +7762,22 @@
         <v>45</v>
       </c>
       <c r="I53" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J53" t="s" s="2">
-        <v>45</v>
+        <v>168</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>425</v>
+        <v>431</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>327</v>
+        <v>432</v>
       </c>
       <c r="N53" t="s" s="2">
-        <v>328</v>
+        <v>182</v>
       </c>
       <c r="O53" t="s" s="2">
         <v>45</v>
@@ -7735,13 +7802,13 @@
         <v>45</v>
       </c>
       <c r="W53" t="s" s="2">
-        <v>45</v>
+        <v>319</v>
       </c>
       <c r="X53" t="s" s="2">
-        <v>45</v>
+        <v>433</v>
       </c>
       <c r="Y53" t="s" s="2">
-        <v>45</v>
+        <v>434</v>
       </c>
       <c r="Z53" t="s" s="2">
         <v>45</v>
@@ -7759,13 +7826,13 @@
         <v>45</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>423</v>
+        <v>429</v>
       </c>
       <c r="AF53" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="AG53" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH53" t="s" s="2">
         <v>45</v>
@@ -7777,23 +7844,499 @@
         <v>45</v>
       </c>
       <c r="AK53" t="s" s="2">
-        <v>45</v>
+        <v>435</v>
       </c>
       <c r="AL53" t="s" s="2">
-        <v>330</v>
+        <v>187</v>
       </c>
       <c r="AM53" t="s" s="2">
-        <v>331</v>
+        <v>188</v>
       </c>
       <c r="AN53" t="s" s="2">
-        <v>45</v>
+        <v>189</v>
       </c>
       <c r="AO53" t="s" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="54" hidden="true">
+      <c r="A54" t="s" s="2">
+        <v>436</v>
+      </c>
+      <c r="B54" s="2"/>
+      <c r="C54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="D54" s="2"/>
+      <c r="E54" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="F54" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="G54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="H54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I54" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="J54" t="s" s="2">
+        <v>275</v>
+      </c>
+      <c r="K54" t="s" s="2">
+        <v>437</v>
+      </c>
+      <c r="L54" t="s" s="2">
+        <v>277</v>
+      </c>
+      <c r="M54" t="s" s="2">
+        <v>438</v>
+      </c>
+      <c r="N54" t="s" s="2">
+        <v>279</v>
+      </c>
+      <c r="O54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="P54" s="2"/>
+      <c r="Q54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="R54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="S54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="X54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Y54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Z54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE54" t="s" s="2">
+        <v>436</v>
+      </c>
+      <c r="AF54" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG54" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AH54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI54" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="AJ54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK54" t="s" s="2">
+        <v>439</v>
+      </c>
+      <c r="AL54" t="s" s="2">
+        <v>282</v>
+      </c>
+      <c r="AM54" t="s" s="2">
+        <v>283</v>
+      </c>
+      <c r="AN54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO54" t="s" s="2">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="55" hidden="true">
+      <c r="A55" t="s" s="2">
+        <v>440</v>
+      </c>
+      <c r="B55" s="2"/>
+      <c r="C55" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="D55" s="2"/>
+      <c r="E55" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="F55" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="G55" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="H55" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I55" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="J55" t="s" s="2">
+        <v>168</v>
+      </c>
+      <c r="K55" t="s" s="2">
+        <v>441</v>
+      </c>
+      <c r="L55" t="s" s="2">
+        <v>442</v>
+      </c>
+      <c r="M55" t="s" s="2">
+        <v>443</v>
+      </c>
+      <c r="N55" t="s" s="2">
+        <v>289</v>
+      </c>
+      <c r="O55" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="P55" s="2"/>
+      <c r="Q55" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="R55" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="S55" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T55" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U55" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V55" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W55" t="s" s="2">
+        <v>290</v>
+      </c>
+      <c r="X55" t="s" s="2">
+        <v>291</v>
+      </c>
+      <c r="Y55" t="s" s="2">
+        <v>292</v>
+      </c>
+      <c r="Z55" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA55" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB55" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC55" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD55" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE55" t="s" s="2">
+        <v>440</v>
+      </c>
+      <c r="AF55" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG55" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AH55" t="s" s="2">
+        <v>293</v>
+      </c>
+      <c r="AI55" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="AJ55" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK55" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL55" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="AM55" t="s" s="2">
+        <v>294</v>
+      </c>
+      <c r="AN55" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO55" t="s" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="56" hidden="true">
+      <c r="A56" t="s" s="2">
+        <v>444</v>
+      </c>
+      <c r="B56" s="2"/>
+      <c r="C56" t="s" s="2">
+        <v>296</v>
+      </c>
+      <c r="D56" s="2"/>
+      <c r="E56" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="F56" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="G56" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="H56" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I56" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="J56" t="s" s="2">
+        <v>168</v>
+      </c>
+      <c r="K56" t="s" s="2">
+        <v>297</v>
+      </c>
+      <c r="L56" t="s" s="2">
+        <v>298</v>
+      </c>
+      <c r="M56" t="s" s="2">
+        <v>299</v>
+      </c>
+      <c r="N56" t="s" s="2">
+        <v>300</v>
+      </c>
+      <c r="O56" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="P56" s="2"/>
+      <c r="Q56" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="R56" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="S56" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T56" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U56" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V56" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W56" t="s" s="2">
+        <v>290</v>
+      </c>
+      <c r="X56" t="s" s="2">
+        <v>301</v>
+      </c>
+      <c r="Y56" t="s" s="2">
+        <v>302</v>
+      </c>
+      <c r="Z56" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA56" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB56" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC56" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD56" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE56" t="s" s="2">
+        <v>444</v>
+      </c>
+      <c r="AF56" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG56" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AH56" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI56" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="AJ56" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK56" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="AL56" t="s" s="2">
+        <v>304</v>
+      </c>
+      <c r="AM56" t="s" s="2">
+        <v>305</v>
+      </c>
+      <c r="AN56" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO56" t="s" s="2">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="57" hidden="true">
+      <c r="A57" t="s" s="2">
+        <v>445</v>
+      </c>
+      <c r="B57" s="2"/>
+      <c r="C57" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="D57" s="2"/>
+      <c r="E57" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="F57" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="G57" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="H57" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I57" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="J57" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="K57" t="s" s="2">
+        <v>446</v>
+      </c>
+      <c r="L57" t="s" s="2">
+        <v>447</v>
+      </c>
+      <c r="M57" t="s" s="2">
+        <v>357</v>
+      </c>
+      <c r="N57" t="s" s="2">
+        <v>358</v>
+      </c>
+      <c r="O57" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="P57" s="2"/>
+      <c r="Q57" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="R57" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="S57" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T57" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U57" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V57" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W57" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="X57" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Y57" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Z57" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA57" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB57" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC57" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD57" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE57" t="s" s="2">
+        <v>445</v>
+      </c>
+      <c r="AF57" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG57" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AH57" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI57" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="AJ57" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK57" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL57" t="s" s="2">
+        <v>360</v>
+      </c>
+      <c r="AM57" t="s" s="2">
+        <v>361</v>
+      </c>
+      <c r="AN57" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO57" t="s" s="2">
         <v>45</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AO53">
+  <autoFilter ref="A1:AO57">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -7803,7 +8346,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI52">
+  <conditionalFormatting sqref="A2:AI56">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Update PriorLevelOfCognitiveFunction and add examples
</commit_message>
<xml_diff>
--- a/build/output/StructureDefinition-pacio-plcf.xlsx
+++ b/build/output/StructureDefinition-pacio-plcf.xlsx
@@ -284,7 +284,7 @@
 </t>
   </si>
   <si>
-    <t>Text summary of the prior level of cognitive function for the patient. (Strongly encouraged to use until more structured method is established)</t>
+    <t>Text summary of the prior level of cognitive function for the patient.</t>
   </si>
   <si>
     <t>A human-readable narrative that contains a summary of the resource and can be used to represent the content of the resource to a human. The narrative need not encode all the structured data, but is required to contain sufficient detail to make it "clinically safe" for a human to just read the narrative. Resource definitions may define what content should be represented in the narrative to ensure clinical safety.</t>
@@ -1593,7 +1593,7 @@
     <col min="8" max="8" width="13.2578125" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="14.44140625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="132.26171875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="104.1484375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -2334,7 +2334,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" hidden="true">
       <c r="A7" t="s" s="2">
         <v>83</v>
       </c>
@@ -2344,13 +2344,13 @@
       </c>
       <c r="D7" s="2"/>
       <c r="E7" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F7" t="s" s="2">
         <v>55</v>
       </c>
       <c r="G7" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="H7" t="s" s="2">
         <v>45</v>

</xml_diff>